<commit_message>
- Fixed bug for new_main.c - Implementing step change in test_sensors.c
</commit_message>
<xml_diff>
--- a/component/Tuning Exp/4-Apr-Tuning.xlsx
+++ b/component/Tuning Exp/4-Apr-Tuning.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MA4012\Rollin-with-a-G\component\Tuning Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58B9658D-7834-431F-9584-631FAE06C668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AEF15E-A1A7-4B85-B4A6-BF3A87F16D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DC43456E-4C53-4D26-8CED-0CFD83C5EF73}"/>
+    <workbookView xWindow="1164" yWindow="6540" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{DC43456E-4C53-4D26-8CED-0CFD83C5EF73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>right IR</t>
   </si>
@@ -53,6 +54,18 @@
   </si>
   <si>
     <t>ln dist</t>
+  </si>
+  <si>
+    <t>right ir</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>left ir</t>
+  </si>
+  <si>
+    <t>ln d</t>
   </si>
 </sst>
 </file>
@@ -1278,6 +1291,728 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$6:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.52945108788915551</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24294617861038939</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10436001532424286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.21072103131565253</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.40047756659712525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$6:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.6026896854443837</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9444389791664403</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1904763503465028</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3672958299864741</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5322256440685598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4514-4C1B-A0F3-C0E66356E7A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="616465272"/>
+        <c:axId val="616464312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="616465272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="616464312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="616464312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="616465272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$16:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.66371836986913313</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43178241642553783</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7658648473814864E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1141943331175213E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-8.3381608939051013E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$16:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.4849066497880004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8903717578961645</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1354942159291497</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3428618046491918</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.520460802488973</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5E49-4CDC-BCDB-004CE5316F82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="419540152"/>
+        <c:axId val="419537592"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="419540152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419537592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="419537592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419540152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1398,6 +2133,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2431,6 +3246,1038 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3051,6 +4898,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0BB8705-D3C4-40B0-907D-3CDCC1EA1532}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DE3CF04-50AB-43F4-A61B-ECF597D353EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3358,8 +5282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EDB859-A3F2-4F70-B52C-079A3AF56A17}">
   <dimension ref="B2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3396,15 +5320,15 @@
         <v>1659</v>
       </c>
       <c r="D3">
-        <f>C3*5/4096</f>
+        <f t="shared" ref="D3:D12" si="0">C3*5/4096</f>
         <v>2.025146484375</v>
       </c>
       <c r="F3">
-        <f>LN(D3)</f>
+        <f t="shared" ref="F3:F12" si="1">LN(D3)</f>
         <v>0.70564203590520114</v>
       </c>
       <c r="G3">
-        <f>LN(B3)</f>
+        <f t="shared" ref="G3:G13" si="2">LN(B3)</f>
         <v>2.4849066497880004</v>
       </c>
       <c r="Q3">
@@ -3423,15 +5347,15 @@
         <v>1400</v>
       </c>
       <c r="D4">
-        <f>C4*5/4096</f>
+        <f t="shared" si="0"/>
         <v>1.708984375</v>
       </c>
       <c r="F4">
-        <f>LN(D4)</f>
+        <f t="shared" si="1"/>
         <v>0.53589926131810661</v>
       </c>
       <c r="G4">
-        <f>LN(B4)</f>
+        <f t="shared" si="2"/>
         <v>2.6390573296152584</v>
       </c>
       <c r="Q4">
@@ -3450,15 +5374,15 @@
         <v>1180</v>
       </c>
       <c r="D5">
-        <f>C5*5/4096</f>
+        <f t="shared" si="0"/>
         <v>1.4404296875</v>
       </c>
       <c r="F5">
-        <f>LN(D5)</f>
+        <f t="shared" si="1"/>
         <v>0.36494146317446713</v>
       </c>
       <c r="G5">
-        <f>LN(B5)</f>
+        <f t="shared" si="2"/>
         <v>2.7725887222397811</v>
       </c>
     </row>
@@ -3470,15 +5394,15 @@
         <v>1110</v>
       </c>
       <c r="D6">
-        <f>C6*5/4096</f>
+        <f t="shared" si="0"/>
         <v>1.35498046875</v>
       </c>
       <c r="F6">
-        <f>LN(D6)</f>
+        <f t="shared" si="1"/>
         <v>0.30378704002113649</v>
       </c>
       <c r="G6">
-        <f>LN(B6)</f>
+        <f t="shared" si="2"/>
         <v>2.8903717578961645</v>
       </c>
     </row>
@@ -3490,15 +5414,15 @@
         <v>1040</v>
       </c>
       <c r="D7">
-        <f>C7*5/4096</f>
+        <f t="shared" si="0"/>
         <v>1.26953125</v>
       </c>
       <c r="F7">
-        <f>LN(D7)</f>
+        <f t="shared" si="1"/>
         <v>0.23864773785017501</v>
       </c>
       <c r="G7">
-        <f>LN(B7)</f>
+        <f t="shared" si="2"/>
         <v>2.9957322735539909</v>
       </c>
     </row>
@@ -3510,15 +5434,15 @@
         <v>865</v>
       </c>
       <c r="D8">
-        <f>C8*5/4096</f>
+        <f t="shared" si="0"/>
         <v>1.055908203125</v>
       </c>
       <c r="F8">
-        <f>LN(D8)</f>
+        <f t="shared" si="1"/>
         <v>5.4401252646635985E-2</v>
       </c>
       <c r="G8">
-        <f>LN(B8)</f>
+        <f t="shared" si="2"/>
         <v>3.0910424533583161</v>
       </c>
     </row>
@@ -3530,15 +5454,15 @@
         <v>782</v>
       </c>
       <c r="D9">
-        <f>C9*5/4096</f>
+        <f t="shared" si="0"/>
         <v>0.95458984375</v>
       </c>
       <c r="F9">
-        <f>LN(D9)</f>
+        <f t="shared" si="1"/>
         <v>-4.6473513739932255E-2</v>
       </c>
       <c r="G9">
-        <f>LN(B9)</f>
+        <f t="shared" si="2"/>
         <v>3.1780538303479458</v>
       </c>
     </row>
@@ -3550,15 +5474,15 @@
         <v>750</v>
       </c>
       <c r="D10">
-        <f>C10*5/4096</f>
+        <f t="shared" si="0"/>
         <v>0.91552734375</v>
       </c>
       <c r="F10">
-        <f>LN(D10)</f>
+        <f t="shared" si="1"/>
         <v>-8.8255047754887211E-2</v>
       </c>
       <c r="G10">
-        <f>LN(B10)</f>
+        <f t="shared" si="2"/>
         <v>3.2580965380214821</v>
       </c>
     </row>
@@ -3570,15 +5494,15 @@
         <v>720</v>
       </c>
       <c r="D11">
-        <f>C11*5/4096</f>
+        <f t="shared" si="0"/>
         <v>0.87890625</v>
       </c>
       <c r="F11">
-        <f>LN(D11)</f>
+        <f t="shared" si="1"/>
         <v>-0.12907704227514236</v>
       </c>
       <c r="G11">
-        <f>LN(B11)</f>
+        <f t="shared" si="2"/>
         <v>3.3322045101752038</v>
       </c>
     </row>
@@ -3590,16 +5514,22 @@
         <v>700</v>
       </c>
       <c r="D12">
-        <f>C12*5/4096</f>
+        <f t="shared" si="0"/>
         <v>0.8544921875</v>
       </c>
       <c r="F12">
-        <f>LN(D12)</f>
+        <f t="shared" si="1"/>
         <v>-0.15724791924183867</v>
       </c>
       <c r="G12">
-        <f>LN(B12)</f>
+        <f t="shared" si="2"/>
         <v>3.4011973816621555</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="G13" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
@@ -3673,15 +5603,15 @@
         <v>1547</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D35" si="0">C24*5/4096</f>
+        <f t="shared" ref="D24:D35" si="3">C24*5/4096</f>
         <v>1.888427734375</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:F35" si="1">LN(D24)</f>
+        <f t="shared" ref="F24:F35" si="4">LN(D24)</f>
         <v>0.63574459628782276</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24:G34" si="2">LN(B24)</f>
+        <f t="shared" ref="G24:G26" si="5">LN(B24)</f>
         <v>2.3025850929940459</v>
       </c>
     </row>
@@ -3693,15 +5623,15 @@
         <v>1175</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.434326171875</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.36069517229301601</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.4849066497880004</v>
       </c>
     </row>
@@ -3713,21 +5643,21 @@
         <v>1065</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.300048828125</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.26240182385828215</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.6390573296152584</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3739,11 +5669,11 @@
         <v>1318</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.60888671875</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.47554246077720919</v>
       </c>
       <c r="G28">
@@ -3759,11 +5689,11 @@
         <v>1128</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.376953125</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.31987317777276086</v>
       </c>
       <c r="G29">
@@ -3779,15 +5709,15 @@
         <v>1035</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.263427734375</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.23382845141422612</v>
       </c>
       <c r="G30">
-        <f t="shared" ref="G30:G35" si="3">LN(B30)</f>
+        <f t="shared" ref="G30:G35" si="6">LN(B30)</f>
         <v>2.9957322735539909</v>
       </c>
     </row>
@@ -3799,15 +5729,15 @@
         <v>945</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.153564453125</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.1428566732084994</v>
       </c>
       <c r="G31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.0910424533583161</v>
       </c>
     </row>
@@ -3819,15 +5749,15 @@
         <v>828</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.0107421875</v>
       </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.0684900100016353E-2</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.1780538303479458</v>
       </c>
     </row>
@@ -3839,15 +5769,15 @@
         <v>797</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.972900390625</v>
       </c>
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.74735754950283E-2</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.2580965380214821</v>
       </c>
     </row>
@@ -3859,15 +5789,15 @@
         <v>763</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.931396484375</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-7.1070223000786331E-2</v>
       </c>
       <c r="G34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.3322045101752038</v>
       </c>
     </row>
@@ -3879,15 +5809,15 @@
         <v>690</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.84228515625</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.17163665669393827</v>
       </c>
       <c r="G35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.4011973816621555</v>
       </c>
     </row>
@@ -3895,6 +5825,234 @@
       <c r="Q37">
         <f>EXP(3.2286)</f>
         <v>25.244290213710194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB10EFA-718D-4ED2-A939-7F820AD46C9B}">
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3">
+        <f>EXP(3.1793)</f>
+        <v>24.029926714658238</v>
+      </c>
+      <c r="R3">
+        <v>-0.9768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1.59</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1.698</v>
+      </c>
+      <c r="B6">
+        <v>13.5</v>
+      </c>
+      <c r="E6">
+        <f>LN(A6)</f>
+        <v>0.52945108788915551</v>
+      </c>
+      <c r="F6">
+        <f>LN(B6)</f>
+        <v>2.6026896854443837</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <f>LN(A7)</f>
+        <v>0.24294617861038939</v>
+      </c>
+      <c r="F7">
+        <f>LN(B7)</f>
+        <v>2.9444389791664403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="B8">
+        <v>24.3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E10" si="0">LN(A8)</f>
+        <v>0.10436001532424286</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F10" si="1">LN(B8)</f>
+        <v>3.1904763503465028</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.81</v>
+      </c>
+      <c r="B9">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>-0.21072103131565253</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>3.3672958299864741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.67</v>
+      </c>
+      <c r="B10">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-0.40047756659712525</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3.5322256440685598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15">
+        <f>EXP(3.3591)</f>
+        <v>28.76329226357657</v>
+      </c>
+      <c r="R15">
+        <v>-1.2682</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1.9419999999999999</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <f>LN(A16)</f>
+        <v>0.66371836986913313</v>
+      </c>
+      <c r="F16">
+        <f>LN(B16)</f>
+        <v>2.4849066497880004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1.54</v>
+      </c>
+      <c r="B17">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <f>LN(A17)</f>
+        <v>0.43178241642553783</v>
+      </c>
+      <c r="F17">
+        <f>LN(B17)</f>
+        <v>2.8903717578961645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1.07</v>
+      </c>
+      <c r="B18">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:E20" si="2">LN(A18)</f>
+        <v>6.7658648473814864E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ref="F18:F20" si="3">LN(B18)</f>
+        <v>3.1354942159291497</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1.042</v>
+      </c>
+      <c r="B19">
+        <v>28.3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>4.1141943331175213E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>3.3428618046491918</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.92</v>
+      </c>
+      <c r="B20">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>-8.3381608939051013E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>3.520460802488973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>